<commit_message>
added & updated screenings
</commit_message>
<xml_diff>
--- a/Consumer Staples - Cosmetics/x_Consumer Staples - Cosmetics.xlsx
+++ b/Consumer Staples - Cosmetics/x_Consumer Staples - Cosmetics.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\simon\Documents\models\Consumer Staples - Cosmetics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8368ABA0-2FB1-440F-92CE-18F1532C91D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E52EB602-2BD5-4FAF-ABA7-66EE7031FECF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-26280" yWindow="-300" windowWidth="24285" windowHeight="13065" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -196,7 +196,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -205,14 +205,11 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="10" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -498,10 +495,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S14"/>
+  <dimension ref="A1:R14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -511,7 +508,6 @@
     <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9" customWidth="1"/>
-    <col min="9" max="9" width="9.140625" style="11"/>
     <col min="10" max="12" width="5.7109375" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="8.5703125" customWidth="1"/>
     <col min="15" max="16" width="6.7109375" bestFit="1" customWidth="1"/>
@@ -519,7 +515,7 @@
     <col min="18" max="18" width="5.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -544,7 +540,7 @@
       <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="10" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
       <c r="J1" s="1" t="s">
@@ -575,7 +571,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>20</v>
       </c>
@@ -600,8 +596,8 @@
       <c r="H2" s="6">
         <v>202306</v>
       </c>
-      <c r="I2" s="15">
-        <v>12.67</v>
+      <c r="I2" s="6">
+        <v>11.06</v>
       </c>
       <c r="J2" s="6">
         <v>0.53</v>
@@ -613,25 +609,31 @@
         <v>0.54</v>
       </c>
       <c r="M2" s="7">
-        <v>-0.15090000000000001</v>
+        <f>K2/J2-1</f>
+        <v>-0.15094339622641506</v>
       </c>
       <c r="N2" s="7">
-        <v>0.2</v>
-      </c>
-      <c r="O2" s="6">
-        <v>28.16</v>
-      </c>
-      <c r="P2" s="6">
-        <v>23.46</v>
+        <f>L2/K2-1</f>
+        <v>0.19999999999999996</v>
+      </c>
+      <c r="O2" s="9">
+        <f>I2/K2</f>
+        <v>24.577777777777779</v>
+      </c>
+      <c r="P2" s="9">
+        <f>I2/L2</f>
+        <v>20.481481481481481</v>
       </c>
       <c r="Q2" s="6">
-        <v>-1.87</v>
+        <f>O2/(M2*100)</f>
+        <v>-1.6282777777777782</v>
       </c>
       <c r="R2" s="6">
-        <v>1.17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+        <f>P2/(N2*100)</f>
+        <v>1.0240740740740741</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>24</v>
       </c>
@@ -656,8 +658,8 @@
       <c r="H3">
         <v>202306</v>
       </c>
-      <c r="I3" s="11">
-        <v>148.83000000000001</v>
+      <c r="I3">
+        <v>144.31</v>
       </c>
       <c r="J3">
         <v>3.46</v>
@@ -668,26 +670,32 @@
       <c r="L3">
         <v>4.18</v>
       </c>
-      <c r="M3" s="2">
-        <v>-0.35260000000000002</v>
-      </c>
-      <c r="N3" s="2">
-        <v>0.86609999999999998</v>
-      </c>
-      <c r="O3">
-        <v>66.44</v>
-      </c>
-      <c r="P3">
-        <v>35.61</v>
-      </c>
-      <c r="Q3">
-        <v>-1.88</v>
-      </c>
-      <c r="R3">
-        <v>0.41</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="M3" s="8">
+        <f t="shared" ref="M3:M7" si="0">K3/J3-1</f>
+        <v>-0.35260115606936404</v>
+      </c>
+      <c r="N3" s="8">
+        <f t="shared" ref="N3:N7" si="1">L3/K3-1</f>
+        <v>0.86607142857142816</v>
+      </c>
+      <c r="O3" s="10">
+        <f t="shared" ref="O3:O7" si="2">I3/K3</f>
+        <v>64.424107142857139</v>
+      </c>
+      <c r="P3" s="10">
+        <f t="shared" ref="P3:P7" si="3">I3/L3</f>
+        <v>34.523923444976077</v>
+      </c>
+      <c r="Q3" s="11">
+        <f t="shared" ref="Q3:Q7" si="4">O3/(M3*100)</f>
+        <v>-1.8271099238875885</v>
+      </c>
+      <c r="R3" s="11">
+        <f t="shared" ref="R3:R7" si="5">P3/(N3*100)</f>
+        <v>0.39862674493168271</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>26</v>
       </c>
@@ -712,8 +720,8 @@
       <c r="H4" s="3">
         <v>202303</v>
       </c>
-      <c r="I4" s="14">
-        <v>217.4</v>
+      <c r="I4" s="3">
+        <v>162.53</v>
       </c>
       <c r="J4" s="3">
         <v>1.66</v>
@@ -725,25 +733,31 @@
         <v>3.54</v>
       </c>
       <c r="M4" s="4">
-        <v>0.83130000000000004</v>
+        <f t="shared" si="0"/>
+        <v>0.8313253012048194</v>
       </c>
       <c r="N4" s="4">
-        <v>0.16450000000000001</v>
-      </c>
-      <c r="O4" s="3">
-        <v>71.510000000000005</v>
-      </c>
-      <c r="P4" s="3">
-        <v>61.41</v>
+        <f t="shared" si="1"/>
+        <v>0.16447368421052633</v>
+      </c>
+      <c r="O4" s="12">
+        <f t="shared" si="2"/>
+        <v>53.463815789473685</v>
+      </c>
+      <c r="P4" s="12">
+        <f t="shared" si="3"/>
+        <v>45.912429378531073</v>
       </c>
       <c r="Q4" s="3">
-        <v>0.86</v>
+        <f t="shared" si="4"/>
+        <v>0.64311546529366881</v>
       </c>
       <c r="R4" s="3">
-        <v>3.73</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>2.7914757062146887</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>28</v>
       </c>
@@ -768,8 +782,8 @@
       <c r="H5">
         <v>202312</v>
       </c>
-      <c r="I5" s="11">
-        <v>145.6</v>
+      <c r="I5">
+        <v>131.27000000000001</v>
       </c>
       <c r="J5">
         <v>4.75</v>
@@ -780,26 +794,32 @@
       <c r="L5">
         <v>5.78</v>
       </c>
-      <c r="M5" s="2">
-        <v>8.6300000000000002E-2</v>
-      </c>
-      <c r="N5" s="2">
-        <v>0.1202</v>
-      </c>
-      <c r="O5">
-        <v>28.22</v>
-      </c>
-      <c r="P5">
-        <v>25.19</v>
-      </c>
-      <c r="Q5">
-        <v>3.27</v>
-      </c>
-      <c r="R5">
-        <v>2.1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="M5" s="8">
+        <f t="shared" si="0"/>
+        <v>8.6315789473684346E-2</v>
+      </c>
+      <c r="N5" s="8">
+        <f t="shared" si="1"/>
+        <v>0.12015503875968991</v>
+      </c>
+      <c r="O5" s="10">
+        <f t="shared" si="2"/>
+        <v>25.439922480620158</v>
+      </c>
+      <c r="P5" s="10">
+        <f t="shared" si="3"/>
+        <v>22.711072664359861</v>
+      </c>
+      <c r="Q5" s="11">
+        <f t="shared" si="4"/>
+        <v>2.9473080922669648</v>
+      </c>
+      <c r="R5" s="11">
+        <f t="shared" si="5"/>
+        <v>1.8901473378725304</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>30</v>
       </c>
@@ -824,8 +844,8 @@
       <c r="H6">
         <v>202312</v>
       </c>
-      <c r="I6" s="11">
-        <v>95.86</v>
+      <c r="I6">
+        <v>89.76</v>
       </c>
       <c r="J6">
         <v>2.61</v>
@@ -836,26 +856,32 @@
       <c r="L6">
         <v>3.02</v>
       </c>
-      <c r="M6" s="2">
-        <v>5.7500000000000002E-2</v>
-      </c>
-      <c r="N6" s="2">
-        <v>9.4200000000000006E-2</v>
-      </c>
-      <c r="O6">
-        <v>34.729999999999997</v>
-      </c>
-      <c r="P6">
-        <v>31.74</v>
-      </c>
-      <c r="Q6">
-        <v>6.04</v>
-      </c>
-      <c r="R6">
-        <v>3.37</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="M6" s="8">
+        <f t="shared" si="0"/>
+        <v>5.7471264367816133E-2</v>
+      </c>
+      <c r="N6" s="8">
+        <f t="shared" si="1"/>
+        <v>9.4202898550724834E-2</v>
+      </c>
+      <c r="O6" s="10">
+        <f t="shared" si="2"/>
+        <v>32.521739130434788</v>
+      </c>
+      <c r="P6" s="10">
+        <f t="shared" si="3"/>
+        <v>29.721854304635762</v>
+      </c>
+      <c r="Q6" s="11">
+        <f t="shared" si="4"/>
+        <v>5.658782608695649</v>
+      </c>
+      <c r="R6" s="11">
+        <f t="shared" si="5"/>
+        <v>3.1550891492613284</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>33</v>
       </c>
@@ -880,8 +906,8 @@
       <c r="H7" s="3">
         <v>202312</v>
       </c>
-      <c r="I7" s="14">
-        <v>27.84</v>
+      <c r="I7" s="3">
+        <v>27.52</v>
       </c>
       <c r="J7" s="3">
         <v>0.39</v>
@@ -893,92 +919,69 @@
         <v>1.38</v>
       </c>
       <c r="M7" s="4">
-        <v>0.4103</v>
+        <f t="shared" si="0"/>
+        <v>0.41025641025641035</v>
       </c>
       <c r="N7" s="4">
-        <v>1.5091000000000001</v>
-      </c>
-      <c r="O7" s="3">
-        <v>50.62</v>
-      </c>
-      <c r="P7" s="3">
-        <v>20.170000000000002</v>
+        <f t="shared" si="1"/>
+        <v>1.5090909090909088</v>
+      </c>
+      <c r="O7" s="12">
+        <f t="shared" si="2"/>
+        <v>50.036363636363632</v>
+      </c>
+      <c r="P7" s="12">
+        <f t="shared" si="3"/>
+        <v>19.942028985507246</v>
       </c>
       <c r="Q7" s="3">
-        <v>1.23</v>
+        <f t="shared" si="4"/>
+        <v>1.2196363636363632</v>
       </c>
       <c r="R7" s="3">
-        <v>0.13</v>
-      </c>
-      <c r="S7" s="8"/>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A9" s="8"/>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8"/>
-      <c r="I9" s="12"/>
-      <c r="J9" s="8"/>
-      <c r="K9" s="8"/>
-      <c r="L9" s="8"/>
-      <c r="M9" s="9">
-        <f>AVERAGE(M2:M7)</f>
-        <v>0.14698333333333333</v>
-      </c>
-      <c r="N9" s="9">
-        <f>AVERAGE(N2:N7)</f>
-        <v>0.49235000000000007</v>
-      </c>
-      <c r="O9" s="13">
-        <f>AVERAGE(O2:O7)</f>
-        <v>46.613333333333337</v>
-      </c>
-      <c r="P9" s="13">
-        <f>AVERAGE(P2:P7)</f>
-        <v>32.93</v>
-      </c>
-      <c r="Q9" s="13">
-        <f>AVERAGE(Q2:Q7)</f>
-        <v>1.2750000000000001</v>
-      </c>
-      <c r="R9" s="13">
-        <f>AVERAGE(R2:R7)</f>
-        <v>1.8183333333333336</v>
-      </c>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A10" s="8"/>
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="8"/>
-      <c r="I10" s="12"/>
-      <c r="J10" s="8"/>
-      <c r="K10" s="8"/>
-      <c r="L10" s="8"/>
-      <c r="M10" s="9"/>
-      <c r="N10" s="9"/>
-      <c r="O10" s="8"/>
-      <c r="P10" s="8"/>
-      <c r="Q10" s="8"/>
-      <c r="R10" s="8"/>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>0.13214597520516852</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="M9" s="2">
+        <f t="shared" ref="M9:R9" si="6">AVERAGE(M2:M7)</f>
+        <v>0.14697070216782518</v>
+      </c>
+      <c r="N9" s="2">
+        <f t="shared" si="6"/>
+        <v>0.49233232653054637</v>
+      </c>
+      <c r="O9" s="5">
+        <f t="shared" si="6"/>
+        <v>41.743954326254531</v>
+      </c>
+      <c r="P9" s="5">
+        <f t="shared" si="6"/>
+        <v>28.882131709915253</v>
+      </c>
+      <c r="Q9" s="5">
+        <f t="shared" si="6"/>
+        <v>1.1689091380378798</v>
+      </c>
+      <c r="R9" s="5">
+        <f t="shared" si="6"/>
+        <v>1.565259831259912</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="M10" s="2"/>
+      <c r="N10" s="2"/>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="M11" s="2"/>
       <c r="N11" s="2"/>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="M12" s="2"/>
       <c r="N12" s="2"/>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="M14" s="2"/>
       <c r="N14" s="2"/>
       <c r="O14" s="5"/>

</xml_diff>